<commit_message>
smote at 2000 samples for logistic change model
</commit_message>
<xml_diff>
--- a/Data/Predictions/Logistic Regression/smote_rating_change_model_2/smote_rating_change_model_2_predictions.xlsx
+++ b/Data/Predictions/Logistic Regression/smote_rating_change_model_2/smote_rating_change_model_2_predictions.xlsx
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2655,7 +2655,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3115,7 +3115,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3375,7 +3375,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3835,7 +3835,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4275,7 +4275,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4415,7 +4415,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Upgrade Since Last Fixed Quarter Date</t>
+          <t>Same As Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4815,7 +4815,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -4855,7 +4855,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5055,7 +5055,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5175,7 +5175,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5295,7 +5295,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5675,7 +5675,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5735,7 +5735,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5915,7 +5915,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5955,7 +5955,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -5995,7 +5995,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6075,7 +6075,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6095,7 +6095,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6235,7 +6235,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6275,7 +6275,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6395,7 +6395,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6515,7 +6515,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6575,7 +6575,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6615,7 +6615,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6655,7 +6655,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6755,7 +6755,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6855,7 +6855,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6895,7 +6895,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -6955,7 +6955,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8255,7 +8255,7 @@
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8355,7 +8355,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8435,7 +8435,7 @@
       </c>
       <c r="D400" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8555,7 +8555,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8615,7 +8615,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8655,7 +8655,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8735,7 +8735,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8795,7 +8795,7 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8895,7 +8895,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -8935,7 +8935,7 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9075,7 +9075,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9215,7 +9215,7 @@
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9255,7 +9255,7 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9275,7 +9275,7 @@
       </c>
       <c r="D442" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9295,7 +9295,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9315,7 +9315,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9415,7 +9415,7 @@
       </c>
       <c r="D449" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9435,7 +9435,7 @@
       </c>
       <c r="D450" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9475,7 +9475,7 @@
       </c>
       <c r="D452" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9535,7 +9535,7 @@
       </c>
       <c r="D455" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9575,7 +9575,7 @@
       </c>
       <c r="D457" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9775,7 +9775,7 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9795,7 +9795,7 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -9875,7 +9875,7 @@
       </c>
       <c r="D472" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10035,7 +10035,7 @@
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10055,7 +10055,7 @@
       </c>
       <c r="D481" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10135,7 +10135,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10335,7 +10335,7 @@
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10355,7 +10355,7 @@
       </c>
       <c r="D496" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10375,7 +10375,7 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10395,7 +10395,7 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10415,7 +10415,7 @@
       </c>
       <c r="D499" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10455,7 +10455,7 @@
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10475,7 +10475,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10815,7 +10815,7 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10835,7 +10835,7 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -10975,7 +10975,7 @@
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11015,7 +11015,7 @@
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11095,7 +11095,7 @@
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11175,7 +11175,7 @@
       </c>
       <c r="D537" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11415,7 +11415,7 @@
       </c>
       <c r="D549" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11455,7 +11455,7 @@
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11715,7 +11715,7 @@
       </c>
       <c r="D564" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11895,7 +11895,7 @@
       </c>
       <c r="D573" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -11935,7 +11935,7 @@
       </c>
       <c r="D575" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12015,7 +12015,7 @@
       </c>
       <c r="D579" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12035,7 +12035,7 @@
       </c>
       <c r="D580" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12055,7 +12055,7 @@
       </c>
       <c r="D581" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12075,7 +12075,7 @@
       </c>
       <c r="D582" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12095,7 +12095,7 @@
       </c>
       <c r="D583" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12175,7 +12175,7 @@
       </c>
       <c r="D587" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12235,7 +12235,7 @@
       </c>
       <c r="D590" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12295,7 +12295,7 @@
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12315,7 +12315,7 @@
       </c>
       <c r="D594" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12375,7 +12375,7 @@
       </c>
       <c r="D597" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12655,7 +12655,7 @@
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12795,7 +12795,7 @@
       </c>
       <c r="D618" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12815,7 +12815,7 @@
       </c>
       <c r="D619" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12855,7 +12855,7 @@
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12875,7 +12875,7 @@
       </c>
       <c r="D622" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12915,7 +12915,7 @@
       </c>
       <c r="D624" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12935,7 +12935,7 @@
       </c>
       <c r="D625" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12955,7 +12955,7 @@
       </c>
       <c r="D626" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -12975,7 +12975,7 @@
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13015,7 +13015,7 @@
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13035,7 +13035,7 @@
       </c>
       <c r="D630" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13055,7 +13055,7 @@
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13135,7 +13135,7 @@
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13155,7 +13155,7 @@
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13215,7 +13215,7 @@
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13255,7 +13255,7 @@
       </c>
       <c r="D641" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13275,7 +13275,7 @@
       </c>
       <c r="D642" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13295,7 +13295,7 @@
       </c>
       <c r="D643" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13315,7 +13315,7 @@
       </c>
       <c r="D644" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13335,7 +13335,7 @@
       </c>
       <c r="D645" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13355,7 +13355,7 @@
       </c>
       <c r="D646" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13375,7 +13375,7 @@
       </c>
       <c r="D647" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13515,7 +13515,7 @@
       </c>
       <c r="D654" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13535,7 +13535,7 @@
       </c>
       <c r="D655" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -13955,7 +13955,7 @@
       </c>
       <c r="D676" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14135,7 +14135,7 @@
       </c>
       <c r="D685" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14315,7 +14315,7 @@
       </c>
       <c r="D694" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14335,7 +14335,7 @@
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14435,7 +14435,7 @@
       </c>
       <c r="D700" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14595,7 +14595,7 @@
       </c>
       <c r="D708" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14715,7 +14715,7 @@
       </c>
       <c r="D714" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14835,7 +14835,7 @@
       </c>
       <c r="D720" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -14855,7 +14855,7 @@
       </c>
       <c r="D721" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15095,7 +15095,7 @@
       </c>
       <c r="D733" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15135,7 +15135,7 @@
       </c>
       <c r="D735" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15195,7 +15195,7 @@
       </c>
       <c r="D738" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15235,7 +15235,7 @@
       </c>
       <c r="D740" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15255,7 +15255,7 @@
       </c>
       <c r="D741" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15355,7 +15355,7 @@
       </c>
       <c r="D746" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15515,7 +15515,7 @@
       </c>
       <c r="D754" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15915,7 +15915,7 @@
       </c>
       <c r="D774" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -15935,7 +15935,7 @@
       </c>
       <c r="D775" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16075,7 +16075,7 @@
       </c>
       <c r="D782" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16115,7 +16115,7 @@
       </c>
       <c r="D784" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16135,7 +16135,7 @@
       </c>
       <c r="D785" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16315,7 +16315,7 @@
       </c>
       <c r="D794" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16335,7 +16335,7 @@
       </c>
       <c r="D795" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16355,7 +16355,7 @@
       </c>
       <c r="D796" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16375,7 +16375,7 @@
       </c>
       <c r="D797" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16395,7 +16395,7 @@
       </c>
       <c r="D798" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16415,7 +16415,7 @@
       </c>
       <c r="D799" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16475,7 +16475,7 @@
       </c>
       <c r="D802" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16535,7 +16535,7 @@
       </c>
       <c r="D805" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16595,7 +16595,7 @@
       </c>
       <c r="D808" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16935,7 +16935,7 @@
       </c>
       <c r="D825" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -16975,7 +16975,7 @@
       </c>
       <c r="D827" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="D829" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17035,7 +17035,7 @@
       </c>
       <c r="D830" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17055,7 +17055,7 @@
       </c>
       <c r="D831" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17075,7 +17075,7 @@
       </c>
       <c r="D832" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17215,7 +17215,7 @@
       </c>
       <c r="D839" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17275,7 +17275,7 @@
       </c>
       <c r="D842" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17375,7 +17375,7 @@
       </c>
       <c r="D847" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17395,7 +17395,7 @@
       </c>
       <c r="D848" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17415,7 +17415,7 @@
       </c>
       <c r="D849" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17495,7 +17495,7 @@
       </c>
       <c r="D853" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17555,7 +17555,7 @@
       </c>
       <c r="D856" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17635,7 +17635,7 @@
       </c>
       <c r="D860" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17735,7 +17735,7 @@
       </c>
       <c r="D865" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17895,7 +17895,7 @@
       </c>
       <c r="D873" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -17935,7 +17935,7 @@
       </c>
       <c r="D875" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18055,7 +18055,7 @@
       </c>
       <c r="D881" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18095,7 +18095,7 @@
       </c>
       <c r="D883" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18115,7 +18115,7 @@
       </c>
       <c r="D884" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18135,7 +18135,7 @@
       </c>
       <c r="D885" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18155,7 +18155,7 @@
       </c>
       <c r="D886" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18175,7 +18175,7 @@
       </c>
       <c r="D887" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18195,7 +18195,7 @@
       </c>
       <c r="D888" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18595,7 +18595,7 @@
       </c>
       <c r="D908" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18675,7 +18675,7 @@
       </c>
       <c r="D912" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18695,7 +18695,7 @@
       </c>
       <c r="D913" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18715,7 +18715,7 @@
       </c>
       <c r="D914" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18735,7 +18735,7 @@
       </c>
       <c r="D915" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18795,7 +18795,7 @@
       </c>
       <c r="D918" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18875,7 +18875,7 @@
       </c>
       <c r="D922" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18895,7 +18895,7 @@
       </c>
       <c r="D923" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18915,7 +18915,7 @@
       </c>
       <c r="D924" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -18995,7 +18995,7 @@
       </c>
       <c r="D928" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19055,7 +19055,7 @@
       </c>
       <c r="D931" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19095,7 +19095,7 @@
       </c>
       <c r="D933" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19135,7 +19135,7 @@
       </c>
       <c r="D935" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19175,7 +19175,7 @@
       </c>
       <c r="D937" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19335,7 +19335,7 @@
       </c>
       <c r="D945" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19375,7 +19375,7 @@
       </c>
       <c r="D947" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19395,7 +19395,7 @@
       </c>
       <c r="D948" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19515,7 +19515,7 @@
       </c>
       <c r="D954" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19635,7 +19635,7 @@
       </c>
       <c r="D960" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19735,7 +19735,7 @@
       </c>
       <c r="D965" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19755,7 +19755,7 @@
       </c>
       <c r="D966" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19815,7 +19815,7 @@
       </c>
       <c r="D969" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19835,7 +19835,7 @@
       </c>
       <c r="D970" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19875,7 +19875,7 @@
       </c>
       <c r="D972" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -19975,7 +19975,7 @@
       </c>
       <c r="D977" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20175,7 +20175,7 @@
       </c>
       <c r="D987" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20275,7 +20275,7 @@
       </c>
       <c r="D992" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20295,7 +20295,7 @@
       </c>
       <c r="D993" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20355,7 +20355,7 @@
       </c>
       <c r="D996" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20375,7 +20375,7 @@
       </c>
       <c r="D997" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20395,7 +20395,7 @@
       </c>
       <c r="D998" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20495,7 +20495,7 @@
       </c>
       <c r="D1003" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20515,7 +20515,7 @@
       </c>
       <c r="D1004" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20535,7 +20535,7 @@
       </c>
       <c r="D1005" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20555,7 +20555,7 @@
       </c>
       <c r="D1006" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20575,7 +20575,7 @@
       </c>
       <c r="D1007" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20595,7 +20595,7 @@
       </c>
       <c r="D1008" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20615,7 +20615,7 @@
       </c>
       <c r="D1009" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20715,7 +20715,7 @@
       </c>
       <c r="D1014" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20835,7 +20835,7 @@
       </c>
       <c r="D1020" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20875,7 +20875,7 @@
       </c>
       <c r="D1022" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -20895,7 +20895,7 @@
       </c>
       <c r="D1023" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21255,7 +21255,7 @@
       </c>
       <c r="D1041" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21275,7 +21275,7 @@
       </c>
       <c r="D1042" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21315,7 +21315,7 @@
       </c>
       <c r="D1044" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21335,7 +21335,7 @@
       </c>
       <c r="D1045" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21355,7 +21355,7 @@
       </c>
       <c r="D1046" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21375,7 +21375,7 @@
       </c>
       <c r="D1047" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21415,7 +21415,7 @@
       </c>
       <c r="D1049" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21595,7 +21595,7 @@
       </c>
       <c r="D1058" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21635,7 +21635,7 @@
       </c>
       <c r="D1060" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21675,7 +21675,7 @@
       </c>
       <c r="D1062" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21695,7 +21695,7 @@
       </c>
       <c r="D1063" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21715,7 +21715,7 @@
       </c>
       <c r="D1064" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21735,7 +21735,7 @@
       </c>
       <c r="D1065" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21755,7 +21755,7 @@
       </c>
       <c r="D1066" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21775,7 +21775,7 @@
       </c>
       <c r="D1067" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21875,7 +21875,7 @@
       </c>
       <c r="D1072" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21915,7 +21915,7 @@
       </c>
       <c r="D1074" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21935,7 +21935,7 @@
       </c>
       <c r="D1075" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21955,7 +21955,7 @@
       </c>
       <c r="D1076" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21975,7 +21975,7 @@
       </c>
       <c r="D1077" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -21995,7 +21995,7 @@
       </c>
       <c r="D1078" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22115,7 +22115,7 @@
       </c>
       <c r="D1084" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22135,7 +22135,7 @@
       </c>
       <c r="D1085" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22235,7 +22235,7 @@
       </c>
       <c r="D1090" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22255,7 +22255,7 @@
       </c>
       <c r="D1091" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22295,7 +22295,7 @@
       </c>
       <c r="D1093" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22515,7 +22515,7 @@
       </c>
       <c r="D1104" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22535,7 +22535,7 @@
       </c>
       <c r="D1105" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22555,7 +22555,7 @@
       </c>
       <c r="D1106" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22595,7 +22595,7 @@
       </c>
       <c r="D1108" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22635,7 +22635,7 @@
       </c>
       <c r="D1110" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Upgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22655,7 +22655,7 @@
       </c>
       <c r="D1111" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22755,7 +22755,7 @@
       </c>
       <c r="D1116" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
@@ -22775,7 +22775,7 @@
       </c>
       <c r="D1117" t="inlineStr">
         <is>
-          <t>Same As Last Fixed Quarter Date</t>
+          <t>Downgrade Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>

</xml_diff>